<commit_message>
updated figure 3 for revision with more random effects in models
</commit_message>
<xml_diff>
--- a/Model_results/compare_2randomeffects_manyrandomeffects_output/Book1.xlsx
+++ b/Model_results/compare_2randomeffects_manyrandomeffects_output/Book1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zoekitchel/Documents/grad_school/Rutgers/Repositories/Col_Ext/Model_results/compare_2randomeffects_manyrandomeffects_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642BFCAB-85BD-B749-AD85-5E6A597118F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E88408-E6F5-FE4F-9028-E403237F65EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{87A85114-4E70-C648-9A39-430FD374C1BD}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="27200" windowHeight="13380" activeTab="2" xr2:uid="{87A85114-4E70-C648-9A39-430FD374C1BD}"/>
   </bookViews>
   <sheets>
     <sheet name="Gains" sheetId="1" r:id="rId1"/>
     <sheet name="Losses" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
   <si>
     <t>variable</t>
   </si>
@@ -94,13 +95,52 @@
   </si>
   <si>
     <t>max_sst_temp_change_lag1_scaled</t>
+  </si>
+  <si>
+    <t>Aleutian Islands</t>
+  </si>
+  <si>
+    <t>Eastern Bering Sea</t>
+  </si>
+  <si>
+    <t>Gulf of Alaska</t>
+  </si>
+  <si>
+    <t>Gulf of Mexico</t>
+  </si>
+  <si>
+    <t>Newfoundland</t>
+  </si>
+  <si>
+    <t>Northeast US</t>
+  </si>
+  <si>
+    <t>Scotian Shelf</t>
+  </si>
+  <si>
+    <t>Southeast US</t>
+  </si>
+  <si>
+    <t>West Coast US</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Total observations</t>
+  </si>
+  <si>
+    <t>Gains</t>
+  </si>
+  <si>
+    <t>Losses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -135,6 +175,12 @@
       <name val="Lucida Grande"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF1C1D1E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -150,10 +196,95 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFFFFFFF"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFFFFFFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -162,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -179,6 +310,27 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,7 +893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF93E8A-1D2B-B647-88F4-523D84AACA4F}">
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -978,4 +1130,622 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B854C9B1-8C4D-B44E-A0C7-E25C758C4B9D}">
+  <dimension ref="A1:N21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:14" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="19">
+        <v>648</v>
+      </c>
+      <c r="C1" s="16">
+        <v>16</v>
+      </c>
+      <c r="D1" s="16">
+        <v>21</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="L1" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="17">
+        <v>2.47E-2</v>
+      </c>
+      <c r="D2" s="17">
+        <v>3.2399999999999998E-2</v>
+      </c>
+      <c r="F2">
+        <f>ROUND(C1/B1,4)*100</f>
+        <v>2.4699999999999998</v>
+      </c>
+      <c r="G2">
+        <f>ROUND(D1/B1,4)*100</f>
+        <v>3.2399999999999998</v>
+      </c>
+      <c r="J2" s="19">
+        <v>408</v>
+      </c>
+      <c r="K2" s="18">
+        <v>7</v>
+      </c>
+      <c r="L2" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="19">
+        <v>3410</v>
+      </c>
+      <c r="C3" s="18">
+        <v>64</v>
+      </c>
+      <c r="D3" s="18">
+        <v>59</v>
+      </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="17">
+        <v>1.72E-2</v>
+      </c>
+      <c r="L3" s="17">
+        <v>1.23E-2</v>
+      </c>
+      <c r="M3">
+        <f>ROUND(K2/$J2,4)*100</f>
+        <v>1.72</v>
+      </c>
+      <c r="N3">
+        <f>ROUND(L2/$J2,4)*100</f>
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="17">
+        <v>1.8800000000000001E-2</v>
+      </c>
+      <c r="D4" s="17">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <f>ROUND(C3/$B3,4)*100</f>
+        <v>1.8800000000000001</v>
+      </c>
+      <c r="G4">
+        <f>ROUND(D3/$B3,4)*100</f>
+        <v>1.73</v>
+      </c>
+      <c r="J4" s="19">
+        <v>1023</v>
+      </c>
+      <c r="K4" s="18">
+        <v>20</v>
+      </c>
+      <c r="L4" s="18">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="19">
+        <v>1274</v>
+      </c>
+      <c r="C5" s="18">
+        <v>44</v>
+      </c>
+      <c r="D5" s="18">
+        <v>8</v>
+      </c>
+      <c r="J5" s="20"/>
+      <c r="K5" s="17">
+        <v>1.9599999999999999E-2</v>
+      </c>
+      <c r="L5" s="17">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ref="M4:M21" si="0">ROUND(K4/$J4,4)*100</f>
+        <v>1.96</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ref="N4:N21" si="1">ROUND(L4/$J4,4)*100</f>
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="17">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="D6" s="17">
+        <v>6.3E-3</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F5:F20" si="2">ROUND(C5/$B5,4)*100</f>
+        <v>3.45</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ref="G5:G20" si="3">ROUND(D5/$B5,4)*100</f>
+        <v>0.63</v>
+      </c>
+      <c r="J6" s="19">
+        <v>715</v>
+      </c>
+      <c r="K6" s="18">
+        <v>8</v>
+      </c>
+      <c r="L6" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="19">
+        <v>2397</v>
+      </c>
+      <c r="C7" s="18">
+        <v>70</v>
+      </c>
+      <c r="D7" s="18">
+        <v>101</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="17">
+        <v>1.12E-2</v>
+      </c>
+      <c r="L7" s="17">
+        <v>8.3999999999999995E-3</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="0"/>
+        <v>1.1199999999999999</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="1"/>
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="17">
+        <v>2.92E-2</v>
+      </c>
+      <c r="D8" s="17">
+        <v>4.2099999999999999E-2</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="2"/>
+        <v>2.92</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="3"/>
+        <v>4.21</v>
+      </c>
+      <c r="J8" s="19">
+        <v>1700</v>
+      </c>
+      <c r="K8" s="18">
+        <v>41</v>
+      </c>
+      <c r="L8" s="18">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="19">
+        <v>1152</v>
+      </c>
+      <c r="C9" s="18">
+        <v>37</v>
+      </c>
+      <c r="D9" s="18">
+        <v>51</v>
+      </c>
+      <c r="J9" s="20"/>
+      <c r="K9" s="17">
+        <v>2.41E-2</v>
+      </c>
+      <c r="L9" s="17">
+        <v>2.41E-2</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="0"/>
+        <v>2.41</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="17">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="D10" s="17">
+        <v>4.4299999999999999E-2</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="2"/>
+        <v>3.2099999999999995</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="3"/>
+        <v>4.43</v>
+      </c>
+      <c r="J10" s="19">
+        <v>608</v>
+      </c>
+      <c r="K10" s="18">
+        <v>15</v>
+      </c>
+      <c r="L10" s="18">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="19">
+        <v>4512</v>
+      </c>
+      <c r="C11" s="18">
+        <v>382</v>
+      </c>
+      <c r="D11" s="18">
+        <v>367</v>
+      </c>
+      <c r="J11" s="20"/>
+      <c r="K11" s="17">
+        <v>2.47E-2</v>
+      </c>
+      <c r="L11" s="17">
+        <v>1.9699999999999999E-2</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="0"/>
+        <v>2.4699999999999998</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="1"/>
+        <v>1.97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="17">
+        <v>8.4699999999999998E-2</v>
+      </c>
+      <c r="D12" s="17">
+        <v>8.1299999999999997E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="2"/>
+        <v>8.4699999999999989</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>8.129999999999999</v>
+      </c>
+      <c r="J12" s="19">
+        <v>3328</v>
+      </c>
+      <c r="K12" s="18">
+        <v>254</v>
+      </c>
+      <c r="L12" s="18">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="19">
+        <v>1968</v>
+      </c>
+      <c r="C13" s="18">
+        <v>122</v>
+      </c>
+      <c r="D13" s="18">
+        <v>121</v>
+      </c>
+      <c r="J13" s="20"/>
+      <c r="K13" s="17">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="L13" s="17">
+        <v>7.2700000000000001E-2</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="0"/>
+        <v>7.6300000000000008</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="1"/>
+        <v>7.2700000000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="17">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0.03</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>6.2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>6.15</v>
+      </c>
+      <c r="J14" s="19">
+        <v>1886</v>
+      </c>
+      <c r="K14" s="18">
+        <v>62</v>
+      </c>
+      <c r="L14" s="18">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="19">
+        <v>2600</v>
+      </c>
+      <c r="C15" s="18">
+        <v>97</v>
+      </c>
+      <c r="D15" s="18">
+        <v>23</v>
+      </c>
+      <c r="J15" s="20"/>
+      <c r="K15" s="17">
+        <v>3.2899999999999999E-2</v>
+      </c>
+      <c r="L15" s="17">
+        <v>3.0200000000000001E-2</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>3.29</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="1"/>
+        <v>3.02</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="17">
+        <v>3.73E-2</v>
+      </c>
+      <c r="D16" s="17">
+        <v>8.8000000000000005E-3</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="2"/>
+        <v>3.73</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>0.88</v>
+      </c>
+      <c r="J16" s="19">
+        <v>1825</v>
+      </c>
+      <c r="K16" s="18">
+        <v>62</v>
+      </c>
+      <c r="L16" s="18">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="19">
+        <v>920</v>
+      </c>
+      <c r="C17" s="18">
+        <v>40</v>
+      </c>
+      <c r="D17" s="18">
+        <v>21</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="17">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="L17" s="17">
+        <v>3.56E-2</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="0"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="N17">
+        <f t="shared" si="1"/>
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="17">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="D18" s="17">
+        <v>2.2800000000000001E-2</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="2"/>
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>2.2800000000000002</v>
+      </c>
+      <c r="J18" s="19">
+        <v>710</v>
+      </c>
+      <c r="K18" s="18">
+        <v>21</v>
+      </c>
+      <c r="L18" s="18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="19">
+        <v>18881</v>
+      </c>
+      <c r="C19" s="18">
+        <v>872</v>
+      </c>
+      <c r="D19" s="18">
+        <v>772</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="17">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="L19" s="17">
+        <v>1.41E-2</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="0"/>
+        <v>2.96</v>
+      </c>
+      <c r="N19">
+        <f t="shared" si="1"/>
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="17">
+        <v>4.6199999999999998E-2</v>
+      </c>
+      <c r="D20" s="17">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="2"/>
+        <v>4.62</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>4.09</v>
+      </c>
+      <c r="J20" s="19">
+        <v>12203</v>
+      </c>
+      <c r="K20" s="18">
+        <v>490</v>
+      </c>
+      <c r="L20" s="18">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="J21" s="20"/>
+      <c r="K21" s="17">
+        <v>4.1700000000000001E-2</v>
+      </c>
+      <c r="L21" s="17">
+        <v>3.8100000000000002E-2</v>
+      </c>
+      <c r="M21">
+        <f>ROUND(K20/$J20,4)*100</f>
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="N21">
+        <f>ROUND(L20/$J20,4)*100</f>
+        <v>3.6799999999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="J6:J7"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>